<commit_message>
Version 3 with it working
</commit_message>
<xml_diff>
--- a/data/bays.xlsx
+++ b/data/bays.xlsx
@@ -430,7 +430,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="str">
-        <v>AC123</v>
+        <v>TYeasd</v>
       </c>
       <c r="D2" t="str">
         <v>Airline 1</v>
@@ -439,7 +439,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <v/>
+        <v>https://www.youtube.com/embed/iQYUlFYt_gE?si=NhYKqK8_dfbNaCs9|https://google.com</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Resolved errors on viewer page
</commit_message>
<xml_diff>
--- a/data/bays.xlsx
+++ b/data/bays.xlsx
@@ -430,16 +430,16 @@
         <v>2</v>
       </c>
       <c r="C2" t="str">
-        <v>56333</v>
+        <v>56888</v>
       </c>
       <c r="D2" t="str">
-        <v>Cars</v>
+        <v>Bay 1 flightline 2</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <v>https://www.youtube.com/embed/iQYUlFYt_gE?si=NhYKqK8_dfbNaCs9|https://www.youtube.com/embed/dQw4w9WgXcQ?si=TGYVlG7oETnDuMSg</v>
+        <v/>
       </c>
     </row>
     <row r="3">
@@ -447,19 +447,19 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="str">
-        <v>cxar</v>
+        <v>Test</v>
       </c>
       <c r="D3" t="str">
-        <v>adada</v>
+        <v>Test</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="str">
-        <v>https://www.youtube.com/embed/iQYUlFYt_gE?si=NhYKqK8_dfbNaCs9|https://example.com/metrics4</v>
+        <v/>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Resolved issues with admin erasing bay info
</commit_message>
<xml_diff>
--- a/data/bays.xlsx
+++ b/data/bays.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,13 +427,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="str">
-        <v>56888</v>
+        <v>teet</v>
       </c>
       <c r="D2" t="str">
-        <v>Bay 1 flightline 2</v>
+        <v>t4etw</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1262,9 +1262,69 @@
         <v>https://example.com/metrics83|https://example.com/metrics84</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Test1</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Test1</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="str">
+        <v>https://www.youtube.com/embed/Ov1v-PxiFMU?autoplay=1&amp;mute=0|https://www.youtube.com/embed/gsIQjyeBC_c?autoplay=1&amp;mute=0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Test2dwadadw</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Test2</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="str">
+        <v>https://www.youtube.com/embed/gsIQjyeBC_c?autoplay=1&amp;mute=0|https://www.youtube.com/embed/dQw4w9WgXcQ?autoplay=1&amp;mute=0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="str">
+        <v>test2</v>
+      </c>
+      <c r="D46" t="str">
+        <v>test2</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46" t="str">
+        <v>https://example.com/metrics3|https://example.com/metrics4</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F43"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F46"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added "Settings" button to allow rotation interval to be updated on admin page.
</commit_message>
<xml_diff>
--- a/data/bays.xlsx
+++ b/data/bays.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1322,9 +1322,29 @@
         <v>https://example.com/metrics3|https://example.com/metrics4</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="str">
+        <v>fssd</v>
+      </c>
+      <c r="D47" t="str">
+        <v>sdf</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F46"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F47"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved issue with header bar overlaping the iframe being displayed.
</commit_message>
<xml_diff>
--- a/data/bays.xlsx
+++ b/data/bays.xlsx
@@ -1270,16 +1270,16 @@
         <v>1</v>
       </c>
       <c r="C44" t="str">
-        <v>Test1</v>
+        <v>56555</v>
       </c>
       <c r="D44" t="str">
-        <v>Test1</v>
+        <v>Bell IT</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44" t="str">
-        <v>https://www.youtube.com/embed/Ov1v-PxiFMU?autoplay=1&amp;mute=0|https://www.youtube.com/embed/gsIQjyeBC_c?autoplay=1&amp;mute=0|https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true</v>
+        <v>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true|https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/IT/BPFIT%20Active%20Projects?rs:embed=true</v>
       </c>
     </row>
     <row r="45">

</xml_diff>

<commit_message>
Setup placeholder for the base url
</commit_message>
<xml_diff>
--- a/data/bays.xlsx
+++ b/data/bays.xlsx
@@ -1,92 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apps\whirlybird\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14A004E-519C-49A1-8285-43804C813C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Bays" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
-  <si>
-    <t>Bay Number</t>
-  </si>
-  <si>
-    <t>Flightline</t>
-  </si>
-  <si>
-    <t>Serial Number</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>URLs</t>
-  </si>
-  <si>
-    <t>teet</t>
-  </si>
-  <si>
-    <t>t4etw</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>56555</t>
-  </si>
-  <si>
-    <t>Bell IT</t>
-  </si>
-  <si>
-    <t>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true|https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/IT/BPFIT%20Active%20Projects?rs:embed=true</t>
-  </si>
-  <si>
-    <t>Test2dwadadw</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/gsIQjyeBC_c?autoplay=1&amp;mute=0|https://www.youtube.com/embed/dQw4w9WgXcQ?autoplay=1&amp;mute=0</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>https://example.com/metrics3|https://example.com/metrics4</t>
-  </si>
-  <si>
-    <t>fssd</t>
-  </si>
-  <si>
-    <t>sdf</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -455,160 +396,155 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD43"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Bay Number</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Flightline</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Serial Number</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Customer Name</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Rank</v>
+      </c>
+      <c r="F1" t="str">
+        <v>URLs</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="C2" t="str">
+        <v>teet</v>
+      </c>
+      <c r="D2" t="str">
+        <v>t4etw</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
+      <c r="C3" t="str">
+        <v>Test</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Test</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
+      <c r="C4" t="str">
+        <v>56555</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Bell IT</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F4" t="str">
+        <v>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true|https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/IT/BPFIT%20Active%20Projects?rs:embed=true</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
+      <c r="C5" t="str">
+        <v>Test2dwadadw</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Test2</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F5" t="str">
+        <v>https://www.youtube.com/embed/gsIQjyeBC_c?autoplay=1&amp;mute=0|https://www.youtube.com/embed/dQw4w9WgXcQ?autoplay=1&amp;mute=0</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
+      <c r="C6" t="str">
+        <v>test2</v>
+      </c>
+      <c r="D6" t="str">
+        <v>test2</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F6" t="str">
+        <v>https://example.com/metrics3|https://example.com/metrics4</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
+      <c r="C7" t="str">
+        <v>fssd</v>
+      </c>
+      <c r="D7" t="str">
+        <v>sdf</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" ht="15.6" x14ac:dyDescent="0.3"/>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F3 A4:F7" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed sidebar and baygrid naming from flightline to Hanger
</commit_message>
<xml_diff>
--- a/data/bays.xlsx
+++ b/data/bays.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -542,9 +542,29 @@
         <v/>
       </c>
     </row>
+    <row r="8">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="str">
+        <v>rwef</v>
+      </c>
+      <c r="D8" t="str">
+        <v>wefwef</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the bay numbering system to maintain compatibility with the existing data structure
</commit_message>
<xml_diff>
--- a/data/bays.xlsx
+++ b/data/bays.xlsx
@@ -397,10 +397,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" customWidth="1" width="10"/>
+    <col min="2" max="2" customWidth="1" width="10"/>
+    <col min="3" max="3" customWidth="1" width="15"/>
+    <col min="4" max="4" customWidth="1" width="20"/>
+    <col min="5" max="5" customWidth="1" width="10"/>
+    <col min="6" max="6" customWidth="1" width="50"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -427,13 +435,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="str">
-        <v>teet</v>
+        <v>56382</v>
       </c>
       <c r="D2" t="str">
-        <v>t4etw</v>
+        <v>Hass</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -444,127 +452,27 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="str">
-        <v>Test</v>
+        <v>56887</v>
       </c>
       <c r="D3" t="str">
-        <v>Test</v>
+        <v>hass bombn</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="str">
-        <v>56555</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Bell IT</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="str">
-        <v>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true|https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/IT/BPFIT%20Active%20Projects?rs:embed=true</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Test2dwadadw</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Test2</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="str">
-        <v>https://www.youtube.com/embed/gsIQjyeBC_c?autoplay=1&amp;mute=0|https://www.youtube.com/embed/dQw4w9WgXcQ?autoplay=1&amp;mute=0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="str">
-        <v>test2</v>
-      </c>
-      <c r="D6" t="str">
-        <v>test2</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" t="str">
-        <v>https://example.com/metrics3|https://example.com/metrics4llll</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7" t="str">
-        <v>fssd</v>
-      </c>
-      <c r="D7" t="str">
-        <v>sdf</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="str">
-        <v>rwef</v>
-      </c>
-      <c r="D8" t="str">
-        <v>wefwef</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed "Invalid bay data" errors
</commit_message>
<xml_diff>
--- a/data/bays.xlsx
+++ b/data/bays.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,7 +415,7 @@
         <v>Bay Number</v>
       </c>
       <c r="B1" t="str">
-        <v>Flightline</v>
+        <v>Hangar</v>
       </c>
       <c r="C1" t="str">
         <v>Serial Number</v>
@@ -431,48 +431,28 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="str">
+        <v>2-1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="str">
-        <v>56382</v>
+        <v>adawd</v>
       </c>
       <c r="D2" t="str">
-        <v>Hass</v>
+        <v>wadawd</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="str">
-        <v>56887</v>
-      </c>
-      <c r="D3" t="str">
-        <v>hass bombn</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" t="str">
-        <v/>
+        <v>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
resolved. The problem was that bay "2-1" belongs to hangar 2, but it was being accessed with hangar=1 in the URL.
</commit_message>
<xml_diff>
--- a/data/bays.xlsx
+++ b/data/bays.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,9 +450,69 @@
         <v>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>2-1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="str">
+        <v>SN123</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Test Customer</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
+        <v>https://example.com/dashboard|https://example.com/status</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>1-1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="str">
+        <v>56887</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Carbo Inc.</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="str">
+        <v>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true|https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>1-1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <v>56887</v>
+      </c>
+      <c r="D5" t="str">
+        <v>hass bombn</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="str">
+        <v>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
End of day version
</commit_message>
<xml_diff>
--- a/data/bays.xlsx
+++ b/data/bays.xlsx
@@ -397,18 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" customWidth="1" width="10"/>
-    <col min="2" max="2" customWidth="1" width="10"/>
-    <col min="3" max="3" customWidth="1" width="15"/>
-    <col min="4" max="4" customWidth="1" width="20"/>
-    <col min="5" max="5" customWidth="1" width="10"/>
-    <col min="6" max="6" customWidth="1" width="50"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -455,19 +447,19 @@
         <v>2-1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="str">
-        <v>SN123</v>
+        <v>adawd</v>
       </c>
       <c r="D3" t="str">
-        <v>Test Customer</v>
+        <v>wadawd</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <v>https://example.com/dashboard|https://example.com/status</v>
+        <v>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true</v>
       </c>
     </row>
     <row r="4">
@@ -487,7 +479,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="str">
-        <v>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true|https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true</v>
+        <v>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true|https://example.com/metrics3</v>
       </c>
     </row>
     <row r="5">
@@ -510,9 +502,29 @@
         <v>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2-2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <v>gsfsfd</v>
+      </c>
+      <c r="D6" t="str">
+        <v>sfsef</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved issue with settings not updating rotation duration.
</commit_message>
<xml_diff>
--- a/data/bays.xlsx
+++ b/data/bays.xlsx
@@ -439,7 +439,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <v>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true</v>
+        <v>https://www.youtube.com/embed/idbUVAw7Gd0?si=nG6eob_oAp7FAk_4|https://www.youtube.com/embed/Jrg9KxGNeJY?si=3HIbZskLyjIhRx4e</v>
       </c>
     </row>
     <row r="3">
@@ -459,7 +459,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <v>https://powerbi.bellflight.com/reports/powerbi/Piney%20Flats/Aircraft%20Services/Part%20Visibility%20Report?rs:embed=true</v>
+        <v>https://www.youtube.com/embed/idbUVAw7Gd0?si=nG6eob_oAp7FAk_4|https://www.youtube.com/embed/Jrg9KxGNeJY?si=3HIbZskLyjIhRx4e</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Fixed bay update issues
</commit_message>
<xml_diff>
--- a/data/bays.xlsx
+++ b/data/bays.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,13 +430,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="str">
-        <v>adawd</v>
+        <v>adawddwdwadwad</v>
       </c>
       <c r="D2" t="str">
         <v>wadawd</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="str">
         <v>https://www.youtube.com/embed/idbUVAw7Gd0?autoplay=1&amp;mute=0|https://www.youtube.com/embed/Jrg9KxGNeJY?si=3HIbZskLyjIhRx4e</v>
@@ -450,13 +450,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="str">
-        <v>adawd</v>
+        <v>adawddwdwadwad</v>
       </c>
       <c r="D3" t="str">
         <v>wadawd</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" t="str">
         <v>https://www.youtube.com/embed/idbUVAw7Gd0?autoplay=1&amp;mute=0|https://www.youtube.com/embed/Jrg9KxGNeJY?si=3HIbZskLyjIhRx4e</v>
@@ -516,15 +516,75 @@
         <v>sfsef</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" t="str">
         <v/>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>4-1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="str">
+        <v>esfe</v>
+      </c>
+      <c r="D7" t="str">
+        <v>efsesf</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>6-2</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="str">
+        <v>sefse</v>
+      </c>
+      <c r="D8" t="str">
+        <v>efssef</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>6-1</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="str">
+        <v>esef</v>
+      </c>
+      <c r="D9" t="str">
+        <v>efsfes</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="str">
+        <v>https://google.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>